<commit_message>
feat: properties for company
</commit_message>
<xml_diff>
--- a/labels.xlsx
+++ b/labels.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28060" windowHeight="13660"/>
+    <workbookView windowWidth="28060" windowHeight="14560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="企业" sheetId="1" r:id="rId1"/>
+    <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144">
   <si>
     <t>原始标签</t>
   </si>
@@ -290,6 +291,162 @@
   </si>
   <si>
     <t>海洋经济龙头企业</t>
+  </si>
+  <si>
+    <t>企业标签</t>
+  </si>
+  <si>
+    <t>企业所处行业</t>
+  </si>
+  <si>
+    <t>金融业</t>
+  </si>
+  <si>
+    <t>交通运输、仓储和邮政业</t>
+  </si>
+  <si>
+    <t>交通运输业</t>
+  </si>
+  <si>
+    <t>仓储业</t>
+  </si>
+  <si>
+    <t>邮政业</t>
+  </si>
+  <si>
+    <t>电力、热力、燃气及水生产和供应业</t>
+  </si>
+  <si>
+    <t>电力生产和供应业</t>
+  </si>
+  <si>
+    <t>热力生产和供应业</t>
+  </si>
+  <si>
+    <t>燃气生产和供应业</t>
+  </si>
+  <si>
+    <t>水生产和供应业</t>
+  </si>
+  <si>
+    <t>批发和零售业</t>
+  </si>
+  <si>
+    <t>批发业</t>
+  </si>
+  <si>
+    <t>零售业</t>
+  </si>
+  <si>
+    <t>水利、环境和公共设施管理业</t>
+  </si>
+  <si>
+    <t>水利业</t>
+  </si>
+  <si>
+    <t>环境业</t>
+  </si>
+  <si>
+    <t>公共设施管理业</t>
+  </si>
+  <si>
+    <t>文化、体育和娱乐业</t>
+  </si>
+  <si>
+    <t>体育业</t>
+  </si>
+  <si>
+    <t>娱乐业</t>
+  </si>
+  <si>
+    <t>文化业</t>
+  </si>
+  <si>
+    <t>卫生和社会工作</t>
+  </si>
+  <si>
+    <t>租赁和商务服务业</t>
+  </si>
+  <si>
+    <t>租赁业</t>
+  </si>
+  <si>
+    <t>商务服务业</t>
+  </si>
+  <si>
+    <t>建筑业</t>
+  </si>
+  <si>
+    <t>国际组织</t>
+  </si>
+  <si>
+    <t>农、林、牧、渔业</t>
+  </si>
+  <si>
+    <t>农业</t>
+  </si>
+  <si>
+    <t>林业</t>
+  </si>
+  <si>
+    <t>牧业</t>
+  </si>
+  <si>
+    <t>渔业</t>
+  </si>
+  <si>
+    <t>居民服务、修理和其他服务业</t>
+  </si>
+  <si>
+    <t>居民服务业</t>
+  </si>
+  <si>
+    <t>修复业</t>
+  </si>
+  <si>
+    <t>其他服务业</t>
+  </si>
+  <si>
+    <t>采矿业</t>
+  </si>
+  <si>
+    <t>住宿和餐饮业</t>
+  </si>
+  <si>
+    <t>住宿业</t>
+  </si>
+  <si>
+    <t>餐饮业</t>
+  </si>
+  <si>
+    <t>教育</t>
+  </si>
+  <si>
+    <t>教育业</t>
+  </si>
+  <si>
+    <t>制造业</t>
+  </si>
+  <si>
+    <t>公共管理、社会保障和社会组织</t>
+  </si>
+  <si>
+    <t>房地产业</t>
+  </si>
+  <si>
+    <t>信息传输、软件和信息技术服务业</t>
+  </si>
+  <si>
+    <t>信息传输业</t>
+  </si>
+  <si>
+    <t>软件业</t>
+  </si>
+  <si>
+    <t>信息技术服务业</t>
+  </si>
+  <si>
+    <t>科学研究和技术服务业</t>
   </si>
 </sst>
 </file>
@@ -297,12 +454,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -311,22 +468,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,6 +497,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -348,26 +512,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -379,17 +535,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,13 +556,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -424,9 +572,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,7 +597,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -448,8 +611,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,37 +634,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,139 +802,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,6 +819,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -691,17 +864,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -719,9 +881,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -740,105 +919,90 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -847,66 +1011,75 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1230,8 +1403,8 @@
   <sheetPr/>
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B$1:B$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>
@@ -1700,4 +1873,700 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:B107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A$1:B$1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="39.4285714285714" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1607142857143" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>